<commit_message>
Drew most of the traces, fixed a few bugs. Timers still broken
</commit_message>
<xml_diff>
--- a/electronics/pinout documentation.xlsx
+++ b/electronics/pinout documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eksia\Documents\Kooliasjad\3. semester\picr22-team-owo\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EB8F6F-E098-4333-B19D-40F89E6A6A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5734829-D323-4C92-A427-6C8EC5835D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11010" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{8091F849-28C4-465A-99B0-8A028E90F78E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8091F849-28C4-465A-99B0-8A028E90F78E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="49">
   <si>
     <t>Timer</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>PF1</t>
+  </si>
+  <si>
+    <t>pre</t>
+  </si>
+  <si>
+    <t>post</t>
   </si>
 </sst>
 </file>
@@ -531,15 +537,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192B8A39-F646-4DE8-AB9A-EA4257792003}">
-  <dimension ref="B1:E26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -552,8 +561,23 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -566,8 +590,20 @@
       <c r="E2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -580,8 +616,20 @@
       <c r="E3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -594,12 +642,26 @@
       <c r="E4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>8</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -612,8 +674,20 @@
       <c r="E6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="1">
+        <v>15</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -626,12 +700,26 @@
       <c r="E7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="1">
+        <v>15</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -644,12 +732,26 @@
       <c r="E9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>3</v>
+      </c>
+      <c r="K9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -662,8 +764,20 @@
       <c r="E11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -676,68 +790,130 @@
       <c r="E12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="H14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="1">
+        <v>3</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2</v>
+      </c>
+      <c r="K15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="1">
+        <v>3</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -750,12 +926,26 @@
       <c r="E18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="1">
+        <v>4</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -766,10 +956,22 @@
         <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="H20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>17</v>
       </c>
@@ -782,8 +984,20 @@
       <c r="E21" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>16</v>
       </c>
@@ -794,10 +1008,22 @@
         <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>19</v>
       </c>
@@ -810,8 +1036,20 @@
       <c r="E23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>20</v>
       </c>
@@ -824,8 +1062,20 @@
       <c r="E24" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>21</v>
       </c>
@@ -838,8 +1088,20 @@
       <c r="E25" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>22</v>
       </c>
@@ -850,6 +1112,18 @@
         <v>39</v>
       </c>
       <c r="E26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed the timer issues (I think)
</commit_message>
<xml_diff>
--- a/electronics/pinout documentation.xlsx
+++ b/electronics/pinout documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eksia\Documents\Kooliasjad\3. semester\picr22-team-owo\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5734829-D323-4C92-A427-6C8EC5835D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C5A2BD-69B4-4E3D-8AC2-C068319409A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8091F849-28C4-465A-99B0-8A028E90F78E}"/>
+    <workbookView xWindow="11010" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{8091F849-28C4-465A-99B0-8A028E90F78E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="50">
   <si>
     <t>Timer</t>
   </si>
@@ -179,10 +179,13 @@
     <t>PF1</t>
   </si>
   <si>
-    <t>pre</t>
-  </si>
-  <si>
-    <t>post</t>
+    <t>ADC1CH2</t>
+  </si>
+  <si>
+    <t>pre fix</t>
+  </si>
+  <si>
+    <t>post fix</t>
   </si>
 </sst>
 </file>
@@ -540,14 +543,14 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -562,7 +565,7 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -736,13 +739,13 @@
         <v>8</v>
       </c>
       <c r="I9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -768,13 +771,13 @@
         <v>9</v>
       </c>
       <c r="I11" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J11" s="1">
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -794,13 +797,13 @@
         <v>10</v>
       </c>
       <c r="I12" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J12" s="1">
         <v>2</v>
       </c>
       <c r="K12" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -929,14 +932,14 @@
       <c r="H18" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="1">
-        <v>4</v>
-      </c>
-      <c r="J18" s="1">
-        <v>1</v>
+      <c r="I18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="K18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
@@ -1020,7 +1023,7 @@
         <v>39</v>
       </c>
       <c r="K22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
@@ -1046,7 +1049,7 @@
         <v>39</v>
       </c>
       <c r="K23" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
@@ -1072,7 +1075,7 @@
         <v>39</v>
       </c>
       <c r="K24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed listed problems, routed power rails, vias currently WIP
</commit_message>
<xml_diff>
--- a/electronics/pinout documentation.xlsx
+++ b/electronics/pinout documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eksia\Documents\Kooliasjad\3. semester\picr22-team-owo\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C5A2BD-69B4-4E3D-8AC2-C068319409A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0910A24D-B912-496B-BBAC-EFCD99F0F0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11010" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{8091F849-28C4-465A-99B0-8A028E90F78E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8091F849-28C4-465A-99B0-8A028E90F78E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="50">
   <si>
     <t>Timer</t>
   </si>
@@ -543,7 +543,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,7 +603,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -629,7 +629,7 @@
         <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1023,7 +1023,7 @@
         <v>39</v>
       </c>
       <c r="K22" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
@@ -1040,7 +1040,7 @@
         <v>43</v>
       </c>
       <c r="H23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>39</v>
@@ -1066,7 +1066,7 @@
         <v>44</v>
       </c>
       <c r="H24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>39</v>
@@ -1075,7 +1075,7 @@
         <v>39</v>
       </c>
       <c r="K24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
@@ -1092,7 +1092,7 @@
         <v>45</v>
       </c>
       <c r="H25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>39</v>
@@ -1101,7 +1101,7 @@
         <v>39</v>
       </c>
       <c r="K25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
@@ -1115,18 +1115,6 @@
         <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
-      </c>
-      <c r="H26" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K26" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed the listed problems, middle 2 planes and reorgnaised traces to create less dead copper.
</commit_message>
<xml_diff>
--- a/electronics/pinout documentation.xlsx
+++ b/electronics/pinout documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eksia\Documents\Kooliasjad\3. semester\picr22-team-owo\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0910A24D-B912-496B-BBAC-EFCD99F0F0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1359B4-1ABE-457C-A06A-90BAD837BC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8091F849-28C4-465A-99B0-8A028E90F78E}"/>
+    <workbookView xWindow="13530" yWindow="-13800" windowWidth="21600" windowHeight="11325" xr2:uid="{8091F849-28C4-465A-99B0-8A028E90F78E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>Timer</t>
   </si>
@@ -95,9 +95,6 @@
     <t>M1D</t>
   </si>
   <si>
-    <t>MOFF</t>
-  </si>
-  <si>
     <t>MSLEEP</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>PA9</t>
   </si>
   <si>
-    <t>PA10</t>
-  </si>
-  <si>
     <t>PB6</t>
   </si>
   <si>
@@ -177,15 +171,6 @@
   </si>
   <si>
     <t>PF1</t>
-  </si>
-  <si>
-    <t>ADC1CH2</t>
-  </si>
-  <si>
-    <t>pre fix</t>
-  </si>
-  <si>
-    <t>post fix</t>
   </si>
 </sst>
 </file>
@@ -540,18 +525,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192B8A39-F646-4DE8-AB9A-EA4257792003}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="B1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -559,28 +541,13 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -593,20 +560,8 @@
       <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -614,25 +569,13 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="1">
-        <v>8</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -640,173 +583,95 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="1">
-        <v>8</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="1">
-        <v>15</v>
-      </c>
-      <c r="J6" s="1">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="1">
-        <v>4</v>
-      </c>
       <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="1">
-        <v>15</v>
-      </c>
-      <c r="J7" s="1">
-        <v>2</v>
-      </c>
-      <c r="K7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="1">
-        <v>3</v>
-      </c>
       <c r="E9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="1">
-        <v>2</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="1">
-        <v>4</v>
-      </c>
-      <c r="J11" s="1">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="1">
-        <v>4</v>
-      </c>
-      <c r="J12" s="1">
-        <v>2</v>
-      </c>
-      <c r="K12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -817,22 +682,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="1">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1">
-        <v>1</v>
-      </c>
-      <c r="K13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -843,22 +696,10 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="1">
-        <v>1</v>
-      </c>
-      <c r="J14" s="1">
-        <v>2</v>
-      </c>
-      <c r="K14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -869,22 +710,10 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="1">
-        <v>3</v>
-      </c>
-      <c r="J15" s="1">
-        <v>2</v>
-      </c>
-      <c r="K15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -895,228 +724,116 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="1">
-        <v>3</v>
-      </c>
-      <c r="J16" s="1">
-        <v>1</v>
-      </c>
-      <c r="K16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="1">
-        <v>4</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
+      <c r="C18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="1"/>
       <c r="E18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
-      </c>
-      <c r="H20" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" t="s">
-        <v>41</v>
-      </c>
-      <c r="H21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
-      </c>
-      <c r="H23" t="s">
-        <v>20</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" t="s">
-        <v>21</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>45</v>
-      </c>
-      <c r="H25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" t="s">
-        <v>46</v>
-      </c>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>